<commit_message>
continue to compute asic control signals and edit pc register read_en
</commit_message>
<xml_diff>
--- a/info/isa.xlsx
+++ b/info/isa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy1\coding\soft_cpu_8b\info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\andy1\repos\cpu_8b\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBE6474-D9FD-4113-B0E5-1D7A31A9E345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC38DC0-DDE2-4B2E-B39C-D26A273CB220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
   </bookViews>
   <sheets>
     <sheet name="asic control signal decode" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="176">
   <si>
     <t>comments</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -677,7 +677,13 @@
     <t>reg_b_write_en</t>
   </si>
   <si>
-    <t>reg_b_read_en</t>
+    <t>reg_b_read_en(only on when reg_b needs to hold the bus)</t>
+  </si>
+  <si>
+    <t>alu_b_sel : reg_b(cpu_bus) 0 / imm 1</t>
+  </si>
+  <si>
+    <t>pc_bus_en</t>
   </si>
 </sst>
 </file>
@@ -984,9 +990,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1024,7 +1030,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1130,7 +1136,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1272,7 +1278,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1280,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A56920-B11D-4893-828B-9E074D852012}">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1295,14 +1301,14 @@
     <col min="10" max="10" width="26.33203125" customWidth="1"/>
     <col min="11" max="11" width="64.21875" customWidth="1"/>
     <col min="12" max="13" width="29" customWidth="1"/>
-    <col min="14" max="14" width="22.33203125" customWidth="1"/>
-    <col min="15" max="15" width="27.44140625" customWidth="1"/>
-    <col min="16" max="16" width="25.44140625" customWidth="1"/>
-    <col min="17" max="17" width="38" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" customWidth="1"/>
+    <col min="14" max="15" width="32.33203125" customWidth="1"/>
+    <col min="16" max="16" width="27.44140625" customWidth="1"/>
+    <col min="17" max="17" width="33" customWidth="1"/>
+    <col min="18" max="18" width="38" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -1346,19 +1352,22 @@
         <v>173</v>
       </c>
       <c r="O1" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="P1" s="19" t="s">
-        <v>169</v>
-      </c>
       <c r="Q1" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1395,13 +1404,13 @@
       <c r="L2" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="M2" s="14"/>
+      <c r="M2" s="14">
+        <v>1</v>
+      </c>
       <c r="N2" s="14">
         <v>1</v>
       </c>
-      <c r="O2" s="14">
-        <v>0</v>
-      </c>
+      <c r="O2" s="14"/>
       <c r="P2" s="14">
         <v>0</v>
       </c>
@@ -1411,8 +1420,11 @@
       <c r="R2" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="S2" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1449,24 +1461,27 @@
       <c r="L3" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="M3" s="14"/>
+      <c r="M3" s="14">
+        <v>1</v>
+      </c>
       <c r="N3" s="14">
-        <v>1</v>
-      </c>
-      <c r="O3" s="14">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O3" s="14"/>
       <c r="P3" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="S3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -1503,13 +1518,13 @@
       <c r="L4" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="M4" s="14"/>
+      <c r="M4" s="14">
+        <v>1</v>
+      </c>
       <c r="N4" s="14">
         <v>1</v>
       </c>
-      <c r="O4" s="14">
-        <v>0</v>
-      </c>
+      <c r="O4" s="14"/>
       <c r="P4" s="14">
         <v>0</v>
       </c>
@@ -1519,8 +1534,11 @@
       <c r="R4" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="S4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -1557,24 +1575,27 @@
       <c r="L5" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="M5" s="14"/>
+      <c r="M5" s="14">
+        <v>1</v>
+      </c>
       <c r="N5" s="14">
-        <v>1</v>
-      </c>
-      <c r="O5" s="14">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O5" s="14"/>
       <c r="P5" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="S5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
@@ -1611,24 +1632,26 @@
       <c r="L6" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="M6" s="14"/>
+      <c r="M6" s="14">
+        <v>1</v>
+      </c>
       <c r="N6" s="14">
         <v>1</v>
       </c>
-      <c r="O6" s="14">
-        <v>0</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="Q6" s="14">
-        <v>0</v>
-      </c>
       <c r="R6" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="S6" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1665,13 +1688,13 @@
       <c r="L7" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="M7" s="14"/>
+      <c r="M7" s="14">
+        <v>1</v>
+      </c>
       <c r="N7" s="14">
         <v>1</v>
       </c>
-      <c r="O7" s="14">
-        <v>0</v>
-      </c>
+      <c r="O7" s="14"/>
       <c r="P7" s="14">
         <v>0</v>
       </c>
@@ -1681,8 +1704,11 @@
       <c r="R7" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="S7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -1719,13 +1745,13 @@
       <c r="L8" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="M8" s="14"/>
+      <c r="M8" s="14">
+        <v>1</v>
+      </c>
       <c r="N8" s="14">
         <v>1</v>
       </c>
-      <c r="O8" s="14">
-        <v>0</v>
-      </c>
+      <c r="O8" s="14"/>
       <c r="P8" s="14">
         <v>0</v>
       </c>
@@ -1735,8 +1761,11 @@
       <c r="R8" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="S8" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -1773,13 +1802,13 @@
       <c r="L9" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="M9" s="14"/>
+      <c r="M9" s="14">
+        <v>1</v>
+      </c>
       <c r="N9" s="14">
         <v>1</v>
       </c>
-      <c r="O9" s="14">
-        <v>0</v>
-      </c>
+      <c r="O9" s="14"/>
       <c r="P9" s="14">
         <v>0</v>
       </c>
@@ -1789,8 +1818,11 @@
       <c r="R9" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="S9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="4" t="s">
         <v>76</v>
       </c>
@@ -1827,24 +1859,27 @@
       <c r="L10" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="M10" s="14"/>
+      <c r="M10" s="14">
+        <v>1</v>
+      </c>
       <c r="N10" s="14">
         <v>1</v>
       </c>
-      <c r="O10" s="14">
-        <v>0</v>
-      </c>
+      <c r="O10" s="14"/>
       <c r="P10" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="Q10" s="14">
-        <v>0</v>
+      <c r="Q10" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="R10" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="S10" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="4" t="s">
         <v>73</v>
       </c>
@@ -1881,24 +1916,27 @@
       <c r="L11" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="M11" s="14"/>
+      <c r="M11" s="14">
+        <v>1</v>
+      </c>
       <c r="N11" s="14">
         <v>1</v>
       </c>
-      <c r="O11" s="14">
-        <v>1</v>
-      </c>
+      <c r="O11" s="14"/>
       <c r="P11" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="Q11" s="14">
-        <v>0</v>
+      <c r="Q11" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="R11" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="S11" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -1935,24 +1973,27 @@
       <c r="L12" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="M12" s="14"/>
+      <c r="M12" s="14">
+        <v>1</v>
+      </c>
       <c r="N12" s="14">
         <v>1</v>
       </c>
-      <c r="O12" s="14">
-        <v>0</v>
-      </c>
-      <c r="P12" s="14" t="s">
+      <c r="O12" s="14"/>
+      <c r="P12" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="Q12" s="14">
-        <v>1</v>
-      </c>
       <c r="R12" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+        <v>1</v>
+      </c>
+      <c r="S12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
@@ -1989,24 +2030,27 @@
       <c r="L13" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="M13" s="14"/>
+      <c r="M13" s="14">
+        <v>0</v>
+      </c>
       <c r="N13" s="14">
-        <v>0</v>
-      </c>
-      <c r="O13" s="14">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="O13" s="14"/>
       <c r="P13" s="14">
         <v>0</v>
       </c>
-      <c r="Q13" s="14" t="s">
+      <c r="Q13" s="14">
+        <v>0</v>
+      </c>
+      <c r="R13" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="R13" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="S13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -2043,24 +2087,27 @@
       <c r="L14" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="M14" s="14"/>
+      <c r="M14" s="14">
+        <v>0</v>
+      </c>
       <c r="N14" s="14">
-        <v>0</v>
-      </c>
-      <c r="O14" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="P14" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="14" t="s">
+      <c r="Q14" s="14">
+        <v>0</v>
+      </c>
+      <c r="R14" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="R14" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="S14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="4" t="s">
         <v>75</v>
       </c>
@@ -2097,24 +2144,27 @@
       <c r="L15" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="M15" s="14"/>
+      <c r="M15" s="14">
+        <v>0</v>
+      </c>
       <c r="N15" s="14">
         <v>0</v>
       </c>
-      <c r="O15" s="14">
-        <v>1</v>
-      </c>
+      <c r="O15" s="14"/>
       <c r="P15" s="14">
         <v>1</v>
       </c>
-      <c r="Q15" s="14" t="s">
+      <c r="Q15" s="14">
+        <v>1</v>
+      </c>
+      <c r="R15" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="R15" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="S15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
@@ -2151,24 +2201,27 @@
       <c r="L16" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="M16" s="14"/>
+      <c r="M16" s="14">
+        <v>0</v>
+      </c>
       <c r="N16" s="14">
-        <v>0</v>
-      </c>
-      <c r="O16" s="14">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="O16" s="14"/>
       <c r="P16" s="14">
         <v>1</v>
       </c>
-      <c r="Q16" s="14" t="s">
+      <c r="Q16" s="14">
+        <v>1</v>
+      </c>
+      <c r="R16" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="R16" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="S16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="4" t="s">
         <v>119</v>
       </c>
@@ -2205,24 +2258,27 @@
       <c r="L17" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="M17" s="14"/>
+      <c r="M17" s="14">
+        <v>0</v>
+      </c>
       <c r="N17" s="14">
-        <v>0</v>
-      </c>
-      <c r="O17" s="14">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="O17" s="14"/>
       <c r="P17" s="14">
         <v>1</v>
       </c>
-      <c r="Q17" s="14" t="s">
+      <c r="Q17" s="14">
+        <v>1</v>
+      </c>
+      <c r="R17" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="R17" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="S17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
@@ -2259,24 +2315,27 @@
       <c r="L18" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="M18" s="14"/>
+      <c r="M18" s="14">
+        <v>0</v>
+      </c>
       <c r="N18" s="14">
-        <v>0</v>
-      </c>
-      <c r="O18" s="14">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="O18" s="14"/>
       <c r="P18" s="14">
         <v>1</v>
       </c>
-      <c r="Q18" s="14" t="s">
+      <c r="Q18" s="14">
+        <v>1</v>
+      </c>
+      <c r="R18" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="R18" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="S18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="4" t="s">
         <v>51</v>
       </c>
@@ -2313,28 +2372,32 @@
       <c r="L19" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="M19" s="14"/>
+      <c r="M19" s="14">
+        <v>0</v>
+      </c>
       <c r="N19" s="14">
-        <v>0</v>
-      </c>
-      <c r="O19" s="14">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="O19" s="14"/>
       <c r="P19" s="14">
         <v>1</v>
       </c>
-      <c r="Q19" s="14" t="s">
+      <c r="Q19" s="14">
+        <v>1</v>
+      </c>
+      <c r="R19" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="R19" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="S19" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="P20" s="15"/>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="20" t="s">
         <v>48</v>
       </c>
@@ -2350,7 +2413,7 @@
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:19">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -2368,7 +2431,7 @@
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:19">
       <c r="A24" s="2">
         <v>2</v>
       </c>
@@ -2386,7 +2449,7 @@
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:19">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -2404,7 +2467,7 @@
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:19">
       <c r="A26" s="2">
         <v>4</v>
       </c>
@@ -2439,7 +2502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B97F70D-B131-4050-83E1-4FBF1CD85DFC}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish asic control signal in excel file and minor edit for asic block diagram
</commit_message>
<xml_diff>
--- a/info/isa.xlsx
+++ b/info/isa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andersonhsieh/repos/cpu_8b/info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF1C87A-2D87-7C4D-A35E-BB76486E97B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA1FE76-9D44-B545-9BB3-45416C0F7753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="176">
   <si>
     <t>comments</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -681,6 +681,9 @@
   </si>
   <si>
     <t>alu_b_sel : reg_b(cpu_bus) 0 / imm 1</t>
+  </si>
+  <si>
+    <t>mem_out_en</t>
   </si>
 </sst>
 </file>
@@ -1283,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A56920-B11D-4893-828B-9E074D852012}">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1302,10 +1305,10 @@
     <col min="15" max="15" width="27.5" customWidth="1"/>
     <col min="16" max="16" width="33" customWidth="1"/>
     <col min="17" max="17" width="38" customWidth="1"/>
-    <col min="18" max="18" width="15.5" customWidth="1"/>
+    <col min="18" max="19" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -1360,8 +1363,11 @@
       <c r="R1" s="19" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S1" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1416,8 +1422,11 @@
       <c r="R2" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S2" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1472,8 +1481,11 @@
       <c r="R3" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -1528,8 +1540,11 @@
       <c r="R4" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -1584,8 +1599,11 @@
       <c r="R5" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
@@ -1640,8 +1658,11 @@
       <c r="R6" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S6" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1696,8 +1717,11 @@
       <c r="R7" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -1752,8 +1776,11 @@
       <c r="R8" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S8" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -1808,8 +1835,11 @@
       <c r="R9" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>76</v>
       </c>
@@ -1864,8 +1894,11 @@
       <c r="R10" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S10" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>73</v>
       </c>
@@ -1920,8 +1953,11 @@
       <c r="R11" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S11" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -1976,8 +2012,11 @@
       <c r="R12" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S12" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
@@ -2032,8 +2071,11 @@
       <c r="R13" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S13" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -2088,8 +2130,11 @@
       <c r="R14" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>75</v>
       </c>
@@ -2144,8 +2189,11 @@
       <c r="R15" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
@@ -2200,8 +2248,11 @@
       <c r="R16" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>119</v>
       </c>
@@ -2256,8 +2307,11 @@
       <c r="R17" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
@@ -2312,8 +2366,11 @@
       <c r="R18" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>51</v>
       </c>
@@ -2368,12 +2425,15 @@
       <c r="R19" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S19" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>48</v>
       </c>
@@ -2389,7 +2449,7 @@
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -2407,7 +2467,7 @@
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>2</v>
       </c>
@@ -2425,7 +2485,7 @@
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -2443,7 +2503,7 @@
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
minor changes in isa.xlsx and worked on white paper
</commit_message>
<xml_diff>
--- a/info/isa.xlsx
+++ b/info/isa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andersonhsieh/repos/cpu_8b/info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA1FE76-9D44-B545-9BB3-45416C0F7753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080D3E1F-68DB-3B4B-A5E8-E58207B80C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="2" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
   </bookViews>
   <sheets>
     <sheet name="asic control signal decode" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="175">
   <si>
     <t>comments</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -516,9 +516,6 @@
   </si>
   <si>
     <t>bge</t>
-  </si>
-  <si>
-    <t># of cycles in single cycle memory design</t>
   </si>
   <si>
     <t>reg_acc = reg_acc + reg_b</t>
@@ -877,7 +874,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -963,6 +960,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1288,18 +1297,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A56920-B11D-4893-828B-9E074D852012}">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView topLeftCell="F1" zoomScale="183" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="H1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="26.33203125" customWidth="1"/>
-    <col min="11" max="11" width="64.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="59" customWidth="1"/>
     <col min="12" max="13" width="29" customWidth="1"/>
     <col min="14" max="14" width="32.33203125" customWidth="1"/>
     <col min="15" max="15" width="27.5" customWidth="1"/>
@@ -1343,28 +1352,28 @@
         <v>57</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M1" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="N1" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="O1" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="P1" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="O1" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="P1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="S1" s="19" t="s">
         <v>174</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="R1" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -1387,22 +1396,22 @@
         <v>33</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M2" s="14">
         <v>1</v>
@@ -1458,10 +1467,10 @@
         <v>46</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M3" s="14">
         <v>1</v>
@@ -1505,22 +1514,22 @@
         <v>33</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M4" s="14">
         <v>1</v>
@@ -1576,10 +1585,10 @@
         <v>47</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M5" s="14">
         <v>1</v>
@@ -1623,22 +1632,22 @@
         <v>33</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M6" s="14">
         <v>1</v>
@@ -1650,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q6" s="14">
         <v>0</v>
@@ -1682,22 +1691,22 @@
         <v>33</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M7" s="14">
         <v>1</v>
@@ -1741,22 +1750,22 @@
         <v>33</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M8" s="14">
         <v>1</v>
@@ -1800,22 +1809,22 @@
         <v>33</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M9" s="14">
         <v>1</v>
@@ -1859,22 +1868,22 @@
         <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>72</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M10" s="14">
         <v>1</v>
@@ -1883,10 +1892,10 @@
         <v>1</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q10" s="14">
         <v>0</v>
@@ -1918,22 +1927,22 @@
         <v>1</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>74</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M11" s="14">
         <v>1</v>
@@ -1945,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q11" s="14">
         <v>0</v>
@@ -1977,22 +1986,22 @@
         <v>33</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M12" s="14">
         <v>1</v>
@@ -2004,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q12" s="14">
         <v>1</v>
@@ -2036,22 +2045,22 @@
         <v>33</v>
       </c>
       <c r="G13" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M13" s="14">
         <v>0</v>
@@ -2066,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R13" s="14">
         <v>1</v>
@@ -2095,22 +2104,22 @@
         <v>33</v>
       </c>
       <c r="G14" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="I14" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M14" s="14">
         <v>0</v>
@@ -2119,13 +2128,13 @@
         <v>1</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P14" s="14">
         <v>0</v>
       </c>
       <c r="Q14" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R14" s="14">
         <v>0</v>
@@ -2169,7 +2178,7 @@
         <v>58</v>
       </c>
       <c r="L15" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M15" s="14">
         <v>0</v>
@@ -2184,7 +2193,7 @@
         <v>1</v>
       </c>
       <c r="Q15" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R15" s="14">
         <v>0</v>
@@ -2213,22 +2222,22 @@
         <v>33</v>
       </c>
       <c r="G16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="I16" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>43</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L16" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M16" s="14">
         <v>0</v>
@@ -2243,7 +2252,7 @@
         <v>1</v>
       </c>
       <c r="Q16" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R16" s="14">
         <v>0</v>
@@ -2272,22 +2281,22 @@
         <v>33</v>
       </c>
       <c r="G17" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H17" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="I17" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>45</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L17" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M17" s="14">
         <v>0</v>
@@ -2302,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="Q17" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R17" s="14">
         <v>0</v>
@@ -2331,22 +2340,22 @@
         <v>0</v>
       </c>
       <c r="G18" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>44</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L18" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M18" s="14">
         <v>0</v>
@@ -2361,7 +2370,7 @@
         <v>1</v>
       </c>
       <c r="Q18" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R18" s="14">
         <v>0</v>
@@ -2390,22 +2399,22 @@
         <v>1</v>
       </c>
       <c r="G19" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="I19" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M19" s="14">
         <v>0</v>
@@ -2420,7 +2429,7 @@
         <v>1</v>
       </c>
       <c r="Q19" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R19" s="14">
         <v>0</v>
@@ -2472,7 +2481,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="23"/>
@@ -2490,7 +2499,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="23"/>
@@ -2538,7 +2547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B97F70D-B131-4050-83E1-4FBF1CD85DFC}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
@@ -2593,22 +2602,22 @@
         <v>57</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M1" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="N1" s="19" t="s">
-        <v>167</v>
-      </c>
       <c r="O1" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q1" s="19" t="s">
         <v>169</v>
-      </c>
-      <c r="P1" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2631,22 +2640,22 @@
         <v>33</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M2" s="14">
         <v>1</v>
@@ -2696,10 +2705,10 @@
         <v>46</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M3" s="14">
         <v>1</v>
@@ -2737,22 +2746,22 @@
         <v>33</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M4" s="14">
         <v>1</v>
@@ -2802,10 +2811,10 @@
         <v>47</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M5" s="14">
         <v>1</v>
@@ -2843,22 +2852,22 @@
         <v>33</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M6" s="14">
         <v>1</v>
@@ -2867,7 +2876,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P6" s="14">
         <v>0</v>
@@ -2896,22 +2905,22 @@
         <v>33</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M7" s="14">
         <v>1</v>
@@ -2949,22 +2958,22 @@
         <v>33</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M8" s="14">
         <v>1</v>
@@ -3002,22 +3011,22 @@
         <v>33</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M9" s="14">
         <v>1</v>
@@ -3055,22 +3064,22 @@
         <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>72</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M10" s="14">
         <v>1</v>
@@ -3079,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P10" s="14">
         <v>0</v>
@@ -3108,22 +3117,22 @@
         <v>1</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>74</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M11" s="14">
         <v>1</v>
@@ -3132,7 +3141,7 @@
         <v>1</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P11" s="14">
         <v>0</v>
@@ -3161,22 +3170,22 @@
         <v>33</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M12" s="14">
         <v>1</v>
@@ -3185,7 +3194,7 @@
         <v>0</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P12" s="14">
         <v>1</v>
@@ -3214,22 +3223,22 @@
         <v>33</v>
       </c>
       <c r="G13" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M13" s="14">
         <v>0</v>
@@ -3241,7 +3250,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q13" s="14">
         <v>1</v>
@@ -3267,34 +3276,34 @@
         <v>33</v>
       </c>
       <c r="G14" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="I14" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M14" s="14">
         <v>0</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O14" s="14">
         <v>0</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q14" s="14">
         <v>0</v>
@@ -3335,7 +3344,7 @@
         <v>58</v>
       </c>
       <c r="L15" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M15" s="14">
         <v>0</v>
@@ -3347,7 +3356,7 @@
         <v>1</v>
       </c>
       <c r="P15" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q15" s="14">
         <v>0</v>
@@ -3373,22 +3382,22 @@
         <v>33</v>
       </c>
       <c r="G16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="I16" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>43</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L16" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M16" s="14">
         <v>0</v>
@@ -3400,7 +3409,7 @@
         <v>1</v>
       </c>
       <c r="P16" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q16" s="14">
         <v>0</v>
@@ -3426,22 +3435,22 @@
         <v>33</v>
       </c>
       <c r="G17" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H17" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="I17" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>45</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L17" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M17" s="14">
         <v>0</v>
@@ -3453,7 +3462,7 @@
         <v>1</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q17" s="14">
         <v>0</v>
@@ -3479,22 +3488,22 @@
         <v>0</v>
       </c>
       <c r="G18" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>44</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L18" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M18" s="14">
         <v>0</v>
@@ -3506,7 +3515,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q18" s="14">
         <v>0</v>
@@ -3532,22 +3541,22 @@
         <v>1</v>
       </c>
       <c r="G19" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="I19" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M19" s="14">
         <v>0</v>
@@ -3559,7 +3568,7 @@
         <v>1</v>
       </c>
       <c r="P19" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q19" s="14">
         <v>0</v>
@@ -3606,7 +3615,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="23"/>
@@ -3623,7 +3632,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="23"/>
@@ -3667,804 +3676,746 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC2C441-DEC2-4001-8CD5-3DBF91AD2891}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K19" sqref="A1:K19"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.33203125" customWidth="1"/>
     <col min="10" max="10" width="26.33203125" customWidth="1"/>
-    <col min="11" max="11" width="64.1640625" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" customWidth="1"/>
-    <col min="13" max="13" width="132.5" customWidth="1"/>
+    <col min="11" max="11" width="48" customWidth="1"/>
+    <col min="12" max="12" width="86.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="29">
+        <v>0</v>
+      </c>
+      <c r="C2" s="29">
+        <v>0</v>
+      </c>
+      <c r="D2" s="29">
+        <v>0</v>
+      </c>
+      <c r="E2" s="29">
+        <v>0</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="13">
-        <v>0</v>
-      </c>
-      <c r="C2" s="13">
-        <v>0</v>
-      </c>
-      <c r="D2" s="13">
-        <v>0</v>
-      </c>
-      <c r="E2" s="13">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="L2" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="29">
+        <v>0</v>
+      </c>
+      <c r="C3" s="29">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29">
+        <v>0</v>
+      </c>
+      <c r="E3" s="29">
+        <v>1</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="29">
+        <v>0</v>
+      </c>
+      <c r="C4" s="29">
+        <v>0</v>
+      </c>
+      <c r="D4" s="29">
+        <v>1</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0</v>
+      </c>
+      <c r="F4" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G4" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I4" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="29">
+        <v>0</v>
+      </c>
+      <c r="C5" s="29">
+        <v>0</v>
+      </c>
+      <c r="D5" s="29">
+        <v>1</v>
+      </c>
+      <c r="E5" s="29">
+        <v>1</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="29">
+        <v>0</v>
+      </c>
+      <c r="C6" s="29">
+        <v>1</v>
+      </c>
+      <c r="D6" s="29">
+        <v>0</v>
+      </c>
+      <c r="E6" s="29">
+        <v>0</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="29">
+        <v>0</v>
+      </c>
+      <c r="C7" s="29">
+        <v>1</v>
+      </c>
+      <c r="D7" s="29">
+        <v>0</v>
+      </c>
+      <c r="E7" s="29">
+        <v>1</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="29">
+        <v>0</v>
+      </c>
+      <c r="C8" s="29">
+        <v>1</v>
+      </c>
+      <c r="D8" s="29">
+        <v>1</v>
+      </c>
+      <c r="E8" s="29">
+        <v>0</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="29">
+        <v>0</v>
+      </c>
+      <c r="C9" s="29">
+        <v>1</v>
+      </c>
+      <c r="D9" s="29">
+        <v>1</v>
+      </c>
+      <c r="E9" s="29">
+        <v>1</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="29">
+        <v>1</v>
+      </c>
+      <c r="C10" s="29">
+        <v>0</v>
+      </c>
+      <c r="D10" s="29">
+        <v>0</v>
+      </c>
+      <c r="E10" s="29">
+        <v>0</v>
+      </c>
+      <c r="F10" s="29">
+        <v>0</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="29">
+        <v>1</v>
+      </c>
+      <c r="C11" s="29">
+        <v>0</v>
+      </c>
+      <c r="D11" s="29">
+        <v>0</v>
+      </c>
+      <c r="E11" s="29">
+        <v>0</v>
+      </c>
+      <c r="F11" s="29">
+        <v>1</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="L2" s="14">
-        <v>1</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="13">
-        <v>0</v>
-      </c>
-      <c r="C3" s="13">
-        <v>0</v>
-      </c>
-      <c r="D3" s="13">
-        <v>0</v>
-      </c>
-      <c r="E3" s="13">
-        <v>1</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="L11" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="29">
+        <v>1</v>
+      </c>
+      <c r="C12" s="29">
+        <v>0</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0</v>
+      </c>
+      <c r="E12" s="29">
+        <v>1</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="29">
+        <v>1</v>
+      </c>
+      <c r="C13" s="29">
+        <v>0</v>
+      </c>
+      <c r="D13" s="29">
+        <v>1</v>
+      </c>
+      <c r="E13" s="29">
+        <v>0</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="29">
+        <v>1</v>
+      </c>
+      <c r="C14" s="29">
+        <v>0</v>
+      </c>
+      <c r="D14" s="29">
+        <v>1</v>
+      </c>
+      <c r="E14" s="29">
+        <v>1</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1</v>
+      </c>
+      <c r="C15" s="29">
+        <v>1</v>
+      </c>
+      <c r="D15" s="29">
+        <v>0</v>
+      </c>
+      <c r="E15" s="29">
+        <v>0</v>
+      </c>
+      <c r="F15" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G15" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H15" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I15" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="L3" s="14">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="13">
-        <v>0</v>
-      </c>
-      <c r="C4" s="13">
-        <v>0</v>
-      </c>
-      <c r="D4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="J15" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="29">
+        <v>1</v>
+      </c>
+      <c r="C16" s="29">
+        <v>1</v>
+      </c>
+      <c r="D16" s="29">
+        <v>0</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G16" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H16" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I16" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="J16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="29">
+        <v>1</v>
+      </c>
+      <c r="C17" s="29">
+        <v>1</v>
+      </c>
+      <c r="D17" s="29">
+        <v>1</v>
+      </c>
+      <c r="E17" s="29">
+        <v>0</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="L4" s="14">
-        <v>1</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="13">
-        <v>0</v>
-      </c>
-      <c r="C5" s="13">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13">
-        <v>1</v>
-      </c>
-      <c r="E5" s="13">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="L5" s="14">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="13">
-        <v>0</v>
-      </c>
-      <c r="C6" s="13">
-        <v>1</v>
-      </c>
-      <c r="D6" s="13">
-        <v>0</v>
-      </c>
-      <c r="E6" s="13">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="H17" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I17" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="L6" s="14">
-        <v>1</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="13">
-        <v>0</v>
-      </c>
-      <c r="C7" s="13">
-        <v>1</v>
-      </c>
-      <c r="D7" s="13">
-        <v>0</v>
-      </c>
-      <c r="E7" s="13">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="J17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="29">
+        <v>1</v>
+      </c>
+      <c r="C18" s="29">
+        <v>1</v>
+      </c>
+      <c r="D18" s="29">
+        <v>1</v>
+      </c>
+      <c r="E18" s="29">
+        <v>1</v>
+      </c>
+      <c r="F18" s="29">
+        <v>0</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I18" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="L7" s="14">
-        <v>1</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="13">
-        <v>0</v>
-      </c>
-      <c r="C8" s="13">
-        <v>1</v>
-      </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="J18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="29">
+        <v>1</v>
+      </c>
+      <c r="C19" s="29">
+        <v>1</v>
+      </c>
+      <c r="D19" s="29">
+        <v>1</v>
+      </c>
+      <c r="E19" s="29">
+        <v>1</v>
+      </c>
+      <c r="F19" s="29">
+        <v>1</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I19" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="L8" s="14">
-        <v>1</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="13">
-        <v>0</v>
-      </c>
-      <c r="C9" s="13">
-        <v>1</v>
-      </c>
-      <c r="D9" s="13">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="L9" s="14">
-        <v>1</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="13">
-        <v>1</v>
-      </c>
-      <c r="C10" s="13">
-        <v>0</v>
-      </c>
-      <c r="D10" s="13">
-        <v>0</v>
-      </c>
-      <c r="E10" s="13">
-        <v>0</v>
-      </c>
-      <c r="F10" s="13">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="L10" s="14">
-        <v>1</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="13">
-        <v>1</v>
-      </c>
-      <c r="C11" s="13">
-        <v>0</v>
-      </c>
-      <c r="D11" s="13">
-        <v>0</v>
-      </c>
-      <c r="E11" s="13">
-        <v>0</v>
-      </c>
-      <c r="F11" s="13">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L11" s="14">
-        <v>1</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="13">
-        <v>1</v>
-      </c>
-      <c r="C12" s="13">
-        <v>0</v>
-      </c>
-      <c r="D12" s="13">
-        <v>0</v>
-      </c>
-      <c r="E12" s="13">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="L12" s="14">
-        <v>2</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="13">
-        <v>0</v>
-      </c>
-      <c r="D13" s="13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="L13" s="14">
-        <v>2</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="13">
-        <v>1</v>
-      </c>
-      <c r="C14" s="13">
-        <v>0</v>
-      </c>
-      <c r="D14" s="13">
-        <v>1</v>
-      </c>
-      <c r="E14" s="13">
-        <v>1</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="L14" s="14">
-        <v>1</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="13">
-        <v>1</v>
-      </c>
-      <c r="C15" s="13">
-        <v>1</v>
-      </c>
-      <c r="D15" s="13">
-        <v>0</v>
-      </c>
-      <c r="E15" s="13">
-        <v>0</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L15" s="14">
-        <v>2</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="13">
-        <v>1</v>
-      </c>
-      <c r="C16" s="13">
-        <v>1</v>
-      </c>
-      <c r="D16" s="13">
-        <v>0</v>
-      </c>
-      <c r="E16" s="13">
-        <v>1</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="L16" s="14">
-        <v>1</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" s="13">
-        <v>1</v>
-      </c>
-      <c r="C17" s="13">
-        <v>1</v>
-      </c>
-      <c r="D17" s="13">
-        <v>1</v>
-      </c>
-      <c r="E17" s="13">
-        <v>0</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="L17" s="14">
-        <v>1</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="13">
-        <v>1</v>
-      </c>
-      <c r="C18" s="13">
-        <v>1</v>
-      </c>
-      <c r="D18" s="13">
-        <v>1</v>
-      </c>
-      <c r="E18" s="13">
-        <v>1</v>
-      </c>
-      <c r="F18" s="13">
-        <v>0</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K18" s="3" t="s">
+      <c r="J19" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="L18" s="14">
-        <v>1</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="13">
-        <v>1</v>
-      </c>
-      <c r="C19" s="13">
-        <v>1</v>
-      </c>
-      <c r="D19" s="13">
-        <v>1</v>
-      </c>
-      <c r="E19" s="13">
-        <v>1</v>
-      </c>
-      <c r="F19" s="13">
-        <v>1</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="L19" s="14">
-        <v>1</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>48</v>
       </c>
@@ -4477,9 +4428,8 @@
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
       <c r="J22" s="22"/>
-      <c r="L22" s="15"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -4494,14 +4444,13 @@
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
       <c r="J23" s="23"/>
-      <c r="L23" s="16"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>2</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="23"/>
@@ -4511,14 +4460,13 @@
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
       <c r="J24" s="23"/>
-      <c r="L24" s="16"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>3</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="23"/>
@@ -4528,9 +4476,8 @@
       <c r="H25" s="23"/>
       <c r="I25" s="23"/>
       <c r="J25" s="23"/>
-      <c r="L25" s="16"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>4</v>
       </c>
@@ -4545,7 +4492,6 @@
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
-      <c r="L26" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>